<commit_message>
modified column names of database
</commit_message>
<xml_diff>
--- a/examples/Aspiration/data/excel_source/trainer_params_scenarios.xlsx
+++ b/examples/Aspiration/data/excel_source/trainer_params_scenarios.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView windowWidth="30240" windowHeight="13040"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
-    <t>training_generation</t>
+    <t>id</t>
+  </si>
+  <si>
+    <t>number_of_path</t>
+  </si>
+  <si>
+    <t>number_of_generation</t>
   </si>
   <si>
     <t>strategy_population</t>
@@ -31,37 +32,34 @@
     <t>mutation_prob</t>
   </si>
   <si>
+    <t>strategy_param_code_length</t>
+  </si>
+  <si>
+    <t>strategy_param_1_min</t>
+  </si>
+  <si>
+    <t>strategy_param_1_max</t>
+  </si>
+  <si>
+    <t>strategy_param_2_min</t>
+  </si>
+  <si>
+    <t>strategy_param_2_max</t>
+  </si>
+  <si>
+    <t>strategy_param_3_min</t>
+  </si>
+  <si>
+    <t>strategy_param_3_max</t>
+  </si>
+  <si>
+    <t>id_scenario</t>
+  </si>
+  <si>
     <t>id_training_scenario</t>
   </si>
   <si>
-    <t>strategy_param_code_length</t>
-  </si>
-  <si>
-    <t>strategy_param_1_min</t>
-  </si>
-  <si>
-    <t>strategy_param_1_max</t>
-  </si>
-  <si>
-    <t>strategy_param_2_min</t>
-  </si>
-  <si>
-    <t>strategy_param_2_max</t>
-  </si>
-  <si>
-    <t>strategy_param_3_min</t>
-  </si>
-  <si>
-    <t>strategy_param_3_max</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>number_of_path</t>
-  </si>
-  <si>
-    <t>id_scenario</t>
+    <t>id_path</t>
   </si>
   <si>
     <t>id_agent</t>
@@ -74,33 +72,373 @@
   </si>
   <si>
     <t>strategy_param_3</t>
-  </si>
-  <si>
-    <t>id_path</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -108,24 +446,310 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="49">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="1" builtinId="52"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="2" builtinId="42"/>
+    <cellStyle name="强调文字颜色 4" xfId="3" builtinId="41"/>
+    <cellStyle name="输入" xfId="4" builtinId="20"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="5" builtinId="39"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="6" builtinId="38"/>
+    <cellStyle name="货币" xfId="7" builtinId="4"/>
+    <cellStyle name="强调文字颜色 3" xfId="8" builtinId="37"/>
+    <cellStyle name="百分比" xfId="9" builtinId="5"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="10" builtinId="36"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="11" builtinId="48"/>
+    <cellStyle name="强调文字颜色 2" xfId="12" builtinId="33"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="13" builtinId="32"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="14" builtinId="44"/>
+    <cellStyle name="计算" xfId="15" builtinId="22"/>
+    <cellStyle name="强调文字颜色 1" xfId="16" builtinId="29"/>
+    <cellStyle name="适中" xfId="17" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="18" builtinId="46"/>
+    <cellStyle name="好" xfId="19" builtinId="26"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="20" builtinId="30"/>
+    <cellStyle name="汇总" xfId="21" builtinId="25"/>
+    <cellStyle name="差" xfId="22" builtinId="27"/>
+    <cellStyle name="检查单元格" xfId="23" builtinId="23"/>
+    <cellStyle name="输出" xfId="24" builtinId="21"/>
+    <cellStyle name="标题 1" xfId="25" builtinId="16"/>
+    <cellStyle name="解释性文本" xfId="26" builtinId="53"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="27" builtinId="34"/>
+    <cellStyle name="标题 4" xfId="28" builtinId="19"/>
+    <cellStyle name="货币[0]" xfId="29" builtinId="7"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="30" builtinId="43"/>
+    <cellStyle name="千位分隔" xfId="31" builtinId="3"/>
+    <cellStyle name="已访问的超链接" xfId="32" builtinId="9"/>
+    <cellStyle name="标题" xfId="33" builtinId="15"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="34" builtinId="35"/>
+    <cellStyle name="警告文本" xfId="35" builtinId="11"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="36" builtinId="40"/>
+    <cellStyle name="注释" xfId="37" builtinId="10"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="38" builtinId="50"/>
+    <cellStyle name="强调文字颜色 5" xfId="39" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51"/>
+    <cellStyle name="超链接" xfId="41" builtinId="8"/>
+    <cellStyle name="千位分隔[0]" xfId="42" builtinId="6"/>
+    <cellStyle name="标题 2" xfId="43" builtinId="17"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
+    <cellStyle name="标题 3" xfId="45" builtinId="18"/>
+    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="47" builtinId="31"/>
+    <cellStyle name="链接单元格" xfId="48" builtinId="24"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -174,7 +798,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -209,7 +833,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -383,86 +1007,81 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.8529411764706" customWidth="1"/>
+    <col min="2" max="2" width="24.1397058823529" customWidth="1"/>
+    <col min="3" max="3" width="17.4264705882353" customWidth="1"/>
+    <col min="4" max="4" width="17.7132352941176" customWidth="1"/>
+    <col min="5" max="5" width="13.5735294117647" customWidth="1"/>
+    <col min="6" max="6" width="27.2867647058824" customWidth="1"/>
+    <col min="7" max="7" width="21.5735294117647" customWidth="1"/>
+    <col min="8" max="8" width="21.8529411764706" customWidth="1"/>
+    <col min="9" max="9" width="18.5735294117647" customWidth="1"/>
+    <col min="10" max="10" width="19" customWidth="1"/>
+    <col min="11" max="11" width="18.5735294117647" customWidth="1"/>
+    <col min="12" max="12" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
-      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D2">
         <v>20</v>
@@ -494,49 +1113,52 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="7" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1397058823529" customWidth="1"/>
+    <col min="2" max="2" width="19.2867647058824" customWidth="1"/>
+    <col min="3" max="3" width="7.71323529411765" customWidth="1"/>
+    <col min="5" max="7" width="16.8529411764706" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
       <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
         <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
analyzer and plotter setup
</commit_message>
<xml_diff>
--- a/examples/Aspiration/data/excel_source/trainer_params_scenarios.xlsx
+++ b/examples/Aspiration/data/excel_source/trainer_params_scenarios.xlsx
@@ -15,7 +15,7 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -392,7 +392,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -454,7 +454,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>50</v>

</xml_diff>

<commit_message>
aspiration example minor revision
</commit_message>
<xml_diff>
--- a/examples/Aspiration/data/excel_source/trainer_params_scenarios.xlsx
+++ b/examples/Aspiration/data/excel_source/trainer_params_scenarios.xlsx
@@ -100,6 +100,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -107,9 +123,107 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -122,120 +236,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -252,73 +252,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -330,103 +414,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -464,6 +464,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -479,11 +499,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -505,32 +531,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -540,142 +540,142 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1009,7 +1009,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1"/>
@@ -1071,7 +1071,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>30</v>

</xml_diff>

<commit_message>
aspiration example muddy analyzer to be cleaned
</commit_message>
<xml_diff>
--- a/examples/Aspiration/data/excel_source/trainer_params_scenarios.xlsx
+++ b/examples/Aspiration/data/excel_source/trainer_params_scenarios.xlsx
@@ -79,10 +79,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -108,24 +108,69 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -139,78 +184,48 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -221,21 +236,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -252,181 +252,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -455,6 +455,36 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -467,8 +497,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -499,159 +529,129 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -660,22 +660,22 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1009,7 +1009,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1"/>

</xml_diff>